<commit_message>
modify build standalone question
</commit_message>
<xml_diff>
--- a/rag_evaluation_results_DaNang.xlsx
+++ b/rag_evaluation_results_DaNang.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,150 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GroundTruth</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Answer</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Faithfulness_Score</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Faithfulness_Explanation</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Relevance_Score</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Relevance_Explanation</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Context_Precision_Score</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Context_Precision_Explanation</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Context_Recall_Score</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Context_Recall_Explanation</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Context_Documents</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Nhà hàng Thìa Gỗ nổi tiếng nhất với món gì?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Thìa Gỗ nổi tiếng với bánh xèo và chả giò, trong đó chả giò giòn rụm, nhẹ, có nhân bò, hải sản hoặc chay.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Nhà hàng Thìa Gỗ nổi tiếng nhất với bánh xèo và chả giò.</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>The answer states that Thìa Gỗ is famous for bánh xèo and chả giò, which is exactly what the provided context says. The answer is fully supported by the context and contains no fabricated or contradictory information.</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>The answer directly states the dishes (bánh xèo and chả giò) that the restaurant is famous for, precisely addressing the question.</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>The context contains a clear statement that Thìa Gỗ is best known for bánh xèo and chả giò, directly supporting the answer. Other documents are irrelevant but do not detract from the precision of the relevant excerpt.</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>The context explicitly states that Thìa Gỗ is famous for bánh xèo and chả giò, and describes chả giò as giòn rụm, nhẹ, with options of bò, hải sản, or chay, matching all key facts in the ground truth.</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Tên tài liệu: 1 Thìa Gỗ Thìa Gỗ là một trong những nhà hàng Đà Nẵng yêu thích của du khách nước ngoài, nổi bật với
-Nội dung: 1 Thìa Gỗ Thìa Gỗ là một trong những nhà hàng Đà Nẵng yêu thích của du khách nước ngoài, nổi bật với ẩm thực Việt mang phong cách gia đình nhưng tinh tế hơn bình thường. Họ có nhiều món truyền thống, nhưng nổi tiếng nhất là bánh xèo và chả giò. Chả giò ở đây giòn rụm, nhẹ, gần như tan ngay khi cắn, có thể chọn nhân bò, hải sản hoặc chay. Bánh xèo to như ở Sài Gòn, vỏ giòn và nhẹ nhưng hơi nhiều dầu. Ngoài ra còn có cơm chiên, rau muống xào, bún bò Nam Bộ
-Tên tài liệu: 25 Nhà Hàng Nổi Tiếng Tại Hà Nội Với Thực Đơn Mới Mẻ, Hấp Dẫn
-Nội dung: 25 Nhà Hàng Nổi Tiếng Tại Hà Nội Với Thực Đơn Mới Mẻ, Hấp Dẫn: Nhà Hàng MIAs Restaurant - Solaria Hotel Hà Nội; 2.Home Hanoi Restaurant Cùng Đại Tiệc Buffet Món Việt Đặc Sắc; 3.Nhà Hàng Nét Huế Hà Nội - Hội Tụ Đặc Sản Miền Trung; 4.Nhà Hàng Vietnamese Cuisine Restaurant - View Hồ Gươm Siêu Thơ Mộng; 5.Nhà Hàng Góc Quê Hà Nội - Đượm Vị Món Truyền Thống Việt; 6.Nhà Hàng Ngự Uyển Hà Nội - Đa Dạng Ẩm Thực Huế; 7.Nhà Hàng Quán Xưa Hà Nội - Cuốn Hút Với Hương Vị Dân Dã; 8.Nhà Hàng Oven d'Or Restaurant
-Tên tài liệu: Nhà Hàng Góc Quê Hà Nội - Đượm Vị Món Truyền Thống Việt
-Nội dung: Nhà Hàng Góc Quê Hà Nội - Đượm Vị Món Truyền Thống Việt: Địa chỉ: 183 Đặng Tiến Đông, Đống Đa, Hà Nội. Nhắc đến các nhà hàng Hà Nội ngon có tiếng thì không thể quên Góc Quê - nhà hàng có điểm đặc trưng là từng món ăn sẽ có những loại nước chấm chuyên biệt. Nếu có cơ hội làm tour ẩm thực Phố cổ Hà Nội thì Góc Quê là một lựa chọn hoàn hảo
-Tên tài liệu: Những nhà hàng Michelin Hà Nội nổi tiếng nhất Việt Nam
-Nội dung: Những nhà hàng Michelin Hà Nội nổi tiếng nhất Việt Nam: Nhà hàng Michelin Hà Nội - Hibana by Koki; Nhà hàng Michelin Hà Nội - Tầm Vị; Nhà hàng Michelin Hà Nội – Gia; Nhà hàng A Bản Mountain Dew; Nhà hàng Akira Back Hà Nội; Nhà hàng Bếp Prime; Nhà hàng Highway 4 (Hàng Tre)
-Tên tài liệu: Nhà hàng Ba Ghien Broken Rice tại 84 Đặng Văn Ngữ, P.10, Q. Phú Nhuận, TP. HCM nổi tiếng với món Bro
-Nội dung: Nhà hàng Ba Ghien Broken Rice tại 84 Đặng Văn Ngữ, P.10, Q. Phú Nhuận, TP. HCM nổi tiếng với món Broken Rice with Grilled Pork Chop (Cơm Tấm Sườn Nướng). Sườn được ướp qua đêm, sau đó nướng trên than để giữ được độ mềm và hương thơm. Món ăn đi kèm với cơm tấm, thịt sườn nướng, chả trứng, bì và nước mắm chua ngọt.
-Tên tài liệu: 2/ Bánh mì Ông Tý Bánh mì ông Tý có thể gọi là món ăn "take-away" nổi tiếng nhất nhì Đà Nẵng. Với sự
-Nội dung: 2/ Bánh mì Ông Tý Bánh mì ông Tý có thể gọi là món ăn "take-away" nổi tiếng nhất nhì Đà Nẵng. Với sự nổi tiếng thế này, chắc hẳn ai cũng nghĩ bánh mì ở đây sẽ phải hoành tráng lắm. Nhưng không, bánh mì Ông Tý chỉ giản dị với topping bao gồm chả bò, chả heo, muối tiêu, ớt bột và một chút bơ. Điều khiến bánh mì Ông Tý được lòng với nhiều khách tới du lịch Đà Nẵng chính là loại chả làm từ thịt tươi, được lọc kỹ gân, da, mỡ
-Tên tài liệu:  Quán Đại Lộc Nổi tiếng với món bánh tráng cuốn thịt heo. Thịt ba chỉ thái mỏng, cuốn cùng nhiều loạ
-Nội dung: Quán Đại Lộc Nổi tiếng với món bánh tráng cuốn thịt heo. Thịt ba chỉ thái mỏng, cuốn cùng nhiều loại rau sống, bún và bánh tráng dẻo. Điểm nhấn là nước chấm mắm nêm – thơm ngon, đậm đà, khó quên. Cách ăn cũng thú vị: nhúng bánh tráng cứng vào nước để mềm ra rồi cuốn cùng nguyên liệu. Quán lúc nào cũng đông khách, có nhiều chi nhánh để lựa chọn. Địa chỉ: 97 Trưng Nữ Vương, Bình Hiên, Hải Châu, Đà Nẵng. Giờ mở cửa: 8:00–21:30. Gợi ý món: Bánh tráng cuốn thịt heo.
-Tên tài liệu: 1 Bánh Xèo Bà Dưỡng Quán nổi tiếng nhất Đà Nẵng về bánh xèo và nem lụi. Bánh xèo ở đây không có nhiề
-Nội dung: 1 Bánh Xèo Bà Dưỡng Quán nổi tiếng nhất Đà Nẵng về bánh xèo và nem lụi. Bánh xèo ở đây không có nhiều lựa chọn nhân, nhưng hương vị cực kỳ ngon, giòn và béo. Nem lụi được làm từ thịt heo băm, nướng trên que sả hoặc tre, ăn cuốn cùng rau và chấm sốt đặc biệt. Đây là một trong những quán được cả người địa phương và du khách yêu thích nhất. Địa chỉ: 280/23 Hoàng Diệu, Bình Hiên, Hải Châu, Đà Nẵng. Giờ mở cửa: 9:30–21:30. Gợi ý món: Bánh xèo, nem lụi.
-Tên tài liệu:  Mỳ Quảng Bà Mua Như đã nói, mì Quảng là món ăn quan trọng nhất trong văn hóa ẩm thực Đà Nẵng. Bạn c
-Nội dung: Mỳ Quảng Bà Mua Như đã nói, mì Quảng là món ăn quan trọng nhất trong văn hóa ẩm thực Đà Nẵng. Bạn có thể tìm thấy quán mì Quảng ở hầu hết các con phố, nhưng một trong những nơi ngon và nổi tiếng nhất là Mỳ Quảng Bà Mua. Ở đây có nhiều loại topping như gà, bò, ếch, trứng… Bát “mì thập cẩm” là lựa chọn tuyệt vời với đủ loại topping trong một phần ăn. Không gian quán thuộc chuỗi nhà hàng khá chỉn chu, phù hợp với ai thích ngồi ăn thoải mái hơn là quán vỉa hè
-Tên tài liệu: Nhà Hàng Vietnamese Cuisine Restaurant - View Hồ Gươm Siêu Thơ Mộng
-Nội dung: . Các món ăn truyền thống của nhà hàng Hà Nội này được chế biến cầu kỳ và trang trí rất công phu, đồng thời được phục vụ trong một không gian mở hiện đại và sang chảnh. Cầu Gỗ mang tới cho cả thực khách trong nước cũng như du khách quốc tế những trải nghiệm vô cùng thoải mái mới lạ.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>